<commit_message>
XGBoost change model 3 with smote 2000
</commit_message>
<xml_diff>
--- a/Data/Predictions/XGBoost/smote_rating_change_model_3/smote_rating_change_model_3_predictions.xlsx
+++ b/Data/Predictions/XGBoost/smote_rating_change_model_3/smote_rating_change_model_3_predictions.xlsx
@@ -2315,7 +2315,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5375,7 +5375,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6275,7 +6275,7 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13155,7 +13155,7 @@
       </c>
       <c r="D636" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18675,7 +18675,7 @@
       </c>
       <c r="D912" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22575,7 +22575,7 @@
       </c>
       <c r="D1107" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22655,7 +22655,7 @@
       </c>
       <c r="D1111" t="inlineStr">
         <is>
-          <t>Downgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>

</xml_diff>